<commit_message>
add results for npb & pwa
</commit_message>
<xml_diff>
--- a/golfgraph/eval.xlsx
+++ b/golfgraph/eval.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smallcat\Documents\GitHub\simgrid\golfgraph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650EF5E5-583F-48DD-9D3D-E62872E5D031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DBBDD1-6D79-4328-99BD-067A35F75E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="516" windowWidth="23040" windowHeight="7728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="execution time (calc2)" sheetId="1" r:id="rId1"/>
+    <sheet name="npb" sheetId="2" r:id="rId2"/>
+    <sheet name="pwa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t>nodes=256, degree=4</t>
     <phoneticPr fontId="1"/>
@@ -74,6 +76,54 @@
     <t>Torus (4*4*4*4)</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>jobs=2000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>turnaround time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Torus-r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Torus-c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Random-c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GolfGraph-c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>utilization</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aspl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>diameter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SDSC-Par</t>
+  </si>
+  <si>
+    <t>NASA-iPSC</t>
+  </si>
+  <si>
+    <t>SDSC-SP2</t>
+  </si>
+  <si>
+    <t>HPC2N</t>
+  </si>
 </sst>
 </file>
 
@@ -115,8 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2536,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2953,4 +3006,444 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09982F2A-1215-4602-876F-BF8471BEAC9C}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="17.796875" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>59.934445304</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.3060469588900001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64.762955805700003</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.1703867355300002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>65.3586683021</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.18414753808</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.25511872581</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <v>6.3605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.24383467668100001</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="1">
+        <v>5.2850000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.24686358176100001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1">
+        <v>5.0860000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883E2438-9E4F-4984-BB6B-C84AD1DBE9FF}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="18.09765625" customWidth="1"/>
+    <col min="2" max="2" width="9.296875" customWidth="1"/>
+    <col min="8" max="8" width="16.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.86717290131</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.101066995489</v>
+      </c>
+      <c r="D4">
+        <v>0.78205910000000001</v>
+      </c>
+      <c r="E4">
+        <v>1.179035397</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2.6619294880500002</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2.4087201491500001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2.3121721974299998</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2.70301829382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>1.167058894</v>
+      </c>
+      <c r="C5">
+        <v>0.11369</v>
+      </c>
+      <c r="D5">
+        <v>0.78056496200000003</v>
+      </c>
+      <c r="E5">
+        <v>1.197854403</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2.7129372722</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2.4924794277700002</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2.2414127180399999</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2.68846217301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1.2133509</v>
+      </c>
+      <c r="C6">
+        <v>0.115423997</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.78401756846799997</v>
+      </c>
+      <c r="E6">
+        <v>1.894479397</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.7328955052200001</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.4853998906300001</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2.2290226425599999</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2.6420209894800002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.25530229369399998</v>
+      </c>
+      <c r="C15">
+        <v>3.7052512309000002E-2</v>
+      </c>
+      <c r="D15">
+        <v>7.3176052256800003E-2</v>
+      </c>
+      <c r="E15">
+        <v>8.5046393993799999E-2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1">
+        <v>4.8145454545500002</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3.8586156111899998</v>
+      </c>
+      <c r="K15" s="1">
+        <v>3.7843137254900001</v>
+      </c>
+      <c r="L15" s="1">
+        <v>4.7884416924700002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.25605356949899999</v>
+      </c>
+      <c r="C16">
+        <v>3.7048795392199997E-2</v>
+      </c>
+      <c r="D16">
+        <v>7.3468317150500007E-2</v>
+      </c>
+      <c r="E16">
+        <v>8.5040987503500004E-2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="1">
+        <v>4.2472727272700004</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3.5655375552300002</v>
+      </c>
+      <c r="K16" s="1">
+        <v>3.1790849673200001</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4.0134158926700003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.25666257466800002</v>
+      </c>
+      <c r="C17">
+        <v>3.7594010828799998E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7.31567003681E-2</v>
+      </c>
+      <c r="E17">
+        <v>8.2639023991600002E-2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4.1987878787900001</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3.3726067746699999</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3.0143790849699998</v>
+      </c>
+      <c r="L17" s="1">
+        <v>3.71104231166</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>